<commit_message>
Fix database Of Data ( Documents )
Sprint 3
</commit_message>
<xml_diff>
--- a/Data/bienban_sprint3/sprint3.xlsx
+++ b/Data/bienban_sprint3/sprint3.xlsx
@@ -1,13 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TranTien\Desktop\CNPM\Data\bienban_sprint3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprint 2" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 3" sheetId="1" r:id="rId1"/>
     <sheet name="CSDL" sheetId="2" r:id="rId2"/>
     <sheet name="Biên bản họp regular Scrum" sheetId="4" r:id="rId3"/>
   </sheets>
@@ -152,7 +157,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -165,7 +170,7 @@
     <font>
       <b/>
       <sz val="16"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -178,14 +183,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -240,12 +245,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -265,6 +264,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -278,6 +283,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -361,43 +369,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:srcRect l="19622" t="18361" r="60759" b="68616"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3505200" y="47625"/>
-          <a:ext cx="2857500" cy="904875"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
       <xdr:row>12</xdr:row>
@@ -417,7 +388,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:srcRect l="19622" t="18492" r="59146" b="59630"/>
         <a:stretch/>
       </xdr:blipFill>
@@ -454,7 +425,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:srcRect l="19724" t="18670" r="57647" b="46998"/>
         <a:stretch/>
       </xdr:blipFill>
@@ -491,7 +462,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:srcRect l="19569" t="18469" r="59531" b="62589"/>
         <a:stretch/>
       </xdr:blipFill>
@@ -499,6 +470,50 @@
         <a:xfrm>
           <a:off x="133350" y="2175164"/>
           <a:ext cx="3037609" cy="1309256"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2924175" y="95250"/>
+          <a:ext cx="3048000" cy="1609725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -553,7 +568,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -588,7 +603,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -803,132 +818,132 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
-    <col min="3" max="3" width="67.140625" customWidth="1"/>
-    <col min="4" max="4" width="66.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.75" customWidth="1"/>
+    <col min="3" max="3" width="67.125" customWidth="1"/>
+    <col min="4" max="4" width="66.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="8"/>
-    </row>
-    <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>7</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -949,11 +964,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="5" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E5" s="1"/>
     </row>
   </sheetData>
@@ -966,19 +981,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -986,63 +1001,63 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="11"/>
+      <c r="B4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="12" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="12" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>31</v>
       </c>
@@ -1050,49 +1065,49 @@
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="11">
         <v>2</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="14" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="12" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="14" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="12" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="14" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="12" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="14" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
@@ -1100,107 +1115,107 @@
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="11">
         <v>3</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="12" t="s">
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="11"/>
+      <c r="B14" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="12" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="11"/>
+      <c r="B15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="12" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="11"/>
+      <c r="B16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="11">
         <v>4</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="12" t="s">
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="11"/>
+      <c r="B18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="12" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="11"/>
+      <c r="B19" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="12" t="s">
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="11"/>
+      <c r="B20" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="13">
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="11">
         <v>5</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="12" t="s">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="11"/>
+      <c r="B22" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="12" t="s">
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
+      <c r="B23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="12" t="s">
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="11"/>
+      <c r="B24" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>